<commit_message>
add project_id column to all references; add WebSite as a new input sheet
</commit_message>
<xml_diff>
--- a/inst/extdata/DSbulkUploadR_input.xlsx
+++ b/inst/extdata/DSbulkUploadR_input.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rlbaker\Rdev_local\DSbulkUploadR\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3FC259B-A180-4D1A-B19A-BE75CD19A3D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="nhB11eCBdRqLSLrm0VCff3XdXVA8GFPLJNdtL+a2W8cxmM/O7BVvdCTkzGyEeGiv3IWQqPzRrR7zk5B3aoDAmw==" workbookSaltValue="fRxFXOBWbRXA1PLpocKcHQ==" workbookSpinCount="100000" lockStructure="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{941BE1E2-8BA7-45DE-88D7-DA0C66FAAF25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="2340" windowWidth="23232" windowHeight="8892" activeTab="1" xr2:uid="{8A6EE447-C162-4970-95C2-F79FBBAD4C55}"/>
+    <workbookView xWindow="984" yWindow="888" windowWidth="21468" windowHeight="8880" activeTab="2" xr2:uid="{8A6EE447-C162-4970-95C2-F79FBBAD4C55}"/>
   </bookViews>
   <sheets>
     <sheet name="AudioRecording" sheetId="1" r:id="rId1"/>
     <sheet name="GenericDocument" sheetId="2" r:id="rId2"/>
+    <sheet name="WebSite" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="41">
   <si>
     <t>reference_type</t>
   </si>
@@ -146,6 +146,21 @@
   </si>
   <si>
     <t>Testing generic document bulk uploads 2</t>
+  </si>
+  <si>
+    <t>project_id</t>
+  </si>
+  <si>
+    <t>WebSite</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Testing web site bulk uploads 1</t>
+  </si>
+  <si>
+    <t>Testing web site bulk uploads 2</t>
   </si>
 </sst>
 </file>
@@ -518,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AA704E2-EB95-4E4A-95B2-36E8F6DDD1DD}">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H10" activeCellId="1" sqref="A4 H10"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -529,7 +544,7 @@
     <col min="5" max="5" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -575,8 +590,11 @@
       <c r="O1" t="s">
         <v>14</v>
       </c>
+      <c r="P1" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -620,7 +638,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -685,10 +703,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32C372F4-B2F9-43E8-90EB-ACDD3F5DA605}">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -696,7 +714,7 @@
     <col min="5" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -739,8 +757,11 @@
       <c r="N1" t="s">
         <v>14</v>
       </c>
+      <c r="O1" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -784,7 +805,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -829,21 +850,182 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="5">
+  <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576" xr:uid="{D995F1AB-73D8-4CCD-B7D1-2F71FF5E8915}">
       <formula1>"GenericDocument"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576" xr:uid="{5B024554-7D2A-46C4-9639-8DBD487DE84E}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576" xr:uid="{4D36C78B-754E-4CA0-B702-72B40F139561}">
-      <formula1>18264</formula1>
-    </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1048576" xr:uid="{1A5FA77B-6383-4CE3-B77A-B252CA9981ED}">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:F1048576" xr:uid="{4D36C78B-754E-4CA0-B702-72B40F139561}">
       <formula1>18264</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K1:K1048576" xr:uid="{4E54745D-EA9D-492A-AE40-2899D961BCFA}">
       <formula1>"1,2,3,4,5"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0591C5C5-FA56-4654-9944-818D77B92433}">
+  <dimension ref="A1:O3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="1">
+        <v>45644</v>
+      </c>
+      <c r="F2" s="1">
+        <v>45646</v>
+      </c>
+      <c r="G2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="1">
+        <v>45636</v>
+      </c>
+      <c r="F3" s="1">
+        <v>45635</v>
+      </c>
+      <c r="G3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>30</v>
+      </c>
+      <c r="M3" t="s">
+        <v>31</v>
+      </c>
+      <c r="N3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K1:K3" xr:uid="{F0505A24-7293-4103-8DBF-E1B56ABCAFED}">
+      <formula1>"1,2,3,4,5"</formula1>
+    </dataValidation>
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:F3" xr:uid="{784B73C4-6D5A-4AA7-A042-5B500BF44D43}">
+      <formula1>18264</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C3" xr:uid="{0786884A-FB50-4BA9-9F50-AD76252D280F}">
+      <formula1>"Yes, No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Reference Type" error="Pleaes inpuut the valid reference type, &quot;WebSite&quot;" sqref="A1:A1048576" xr:uid="{69D49FC2-74B6-48C0-8D1D-DBD2A221AA55}">
+      <formula1>"WebSite"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add CUI markings, CUI contact name, and CUI email address fields.
</commit_message>
<xml_diff>
--- a/inst/extdata/DSbulkUploadR_input.xlsx
+++ b/inst/extdata/DSbulkUploadR_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rlbaker\Rdev_local\DSbulkUploadR\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{614167E1-8868-4546-BA35-E5CAC303684E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F32EC832-CB93-4B6F-9267-B89AEA4BB086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31620" yWindow="3915" windowWidth="21465" windowHeight="8880" activeTab="1" xr2:uid="{8A6EE447-C162-4970-95C2-F79FBBAD4C55}"/>
+    <workbookView xWindow="32565" yWindow="4605" windowWidth="21465" windowHeight="8880" activeTab="2" xr2:uid="{8A6EE447-C162-4970-95C2-F79FBBAD4C55}"/>
   </bookViews>
   <sheets>
     <sheet name="AudioRecording" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="57">
   <si>
     <t>reference_type</t>
   </si>
@@ -170,16 +170,63 @@
   </si>
   <si>
     <t>https://www.google.com</t>
+  </si>
+  <si>
+    <t>PUBLIC</t>
+  </si>
+  <si>
+    <t>CUI_label</t>
+  </si>
+  <si>
+    <t>Criminal History Record Information</t>
+  </si>
+  <si>
+    <t>Smoky T. Bear</t>
+  </si>
+  <si>
+    <t>Rod Stewart</t>
+  </si>
+  <si>
+    <t>CUI_contact_email</t>
+  </si>
+  <si>
+    <t>CUI_contact_name</t>
+  </si>
+  <si>
+    <t>nps@nps.gov</t>
+  </si>
+  <si>
+    <t>NRSS_DataStore@nps.gov</t>
+  </si>
+  <si>
+    <t>Somehow differs from description. Or not.</t>
+  </si>
+  <si>
+    <t>nothing noteworthy.</t>
+  </si>
+  <si>
+    <t>nothing of note.</t>
+  </si>
+  <si>
+    <t>NRSS, IMD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -202,14 +249,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -542,19 +592,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AA704E2-EB95-4E4A-95B2-36E8F6DDD1DD}">
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="12.6640625" customWidth="1"/>
-    <col min="6" max="6" width="18.33203125" customWidth="1"/>
+    <col min="1" max="1" width="13.21875" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" customWidth="1"/>
+    <col min="8" max="8" width="10.21875" customWidth="1"/>
+    <col min="10" max="10" width="6.33203125" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" customWidth="1"/>
+    <col min="12" max="12" width="11.77734375" customWidth="1"/>
+    <col min="14" max="14" width="10.6640625" customWidth="1"/>
+    <col min="18" max="18" width="9.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -592,19 +650,28 @@
         <v>11</v>
       </c>
       <c r="M1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N1" t="s">
+        <v>50</v>
+      </c>
+      <c r="O1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -612,7 +679,7 @@
         <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s">
         <v>18</v>
@@ -630,25 +697,37 @@
         <v>20</v>
       </c>
       <c r="I2" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="J2" t="s">
+        <v>54</v>
+      </c>
+      <c r="K2" t="s">
         <v>22</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>1</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
+        <v>44</v>
+      </c>
+      <c r="N2" t="s">
+        <v>47</v>
+      </c>
+      <c r="O2" t="s">
+        <v>51</v>
+      </c>
+      <c r="P2" t="s">
         <v>23</v>
       </c>
-      <c r="M2" t="s">
+      <c r="Q2" t="s">
         <v>24</v>
       </c>
-      <c r="N2" t="s">
+      <c r="R2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -674,57 +753,70 @@
         <v>20</v>
       </c>
       <c r="I3" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="J3" t="s">
+        <v>55</v>
+      </c>
+      <c r="K3" t="s">
         <v>29</v>
       </c>
-      <c r="K3">
-        <v>1</v>
-      </c>
-      <c r="L3" t="s">
-        <v>30</v>
+      <c r="L3">
+        <v>2</v>
       </c>
       <c r="M3" t="s">
+        <v>46</v>
+      </c>
+      <c r="N3" t="s">
+        <v>48</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="P3" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q3" t="s">
         <v>31</v>
       </c>
-      <c r="N3" t="s">
+      <c r="R3" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="4">
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Enter Yes or No" sqref="C1:C1048576" xr:uid="{DE3F3B79-935D-49B3-B6E5-2FDC28265CA8}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:F1048576" xr:uid="{DA4EDB11-3D2C-4C90-B480-E65029AEF54D}">
       <formula1>18264</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L1:L1048576" xr:uid="{0671E3C4-598D-4EC6-A109-8DB7168E5C3E}">
-      <formula1>"1, 2, 3, 4, 5"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Data" error="Please choose a valid data type" sqref="A1:A1048576" xr:uid="{ECEDD389-5EA6-40DC-B00D-DD1E340A604A}">
       <formula1>"AudioRecording"</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="O3" r:id="rId1" display="mailto:NRSS_DataStore@nps.gov" xr:uid="{3E3AFA6B-8503-44EF-BF3A-F5429543D37C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32C372F4-B2F9-43E8-90EB-ACDD3F5DA605}">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:O3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:N1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="5" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -759,19 +851,28 @@
         <v>11</v>
       </c>
       <c r="L1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M1" t="s">
+        <v>50</v>
+      </c>
+      <c r="N1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O1" t="s">
         <v>12</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>13</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>14</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -806,16 +907,25 @@
         <v>1</v>
       </c>
       <c r="L2" t="s">
+        <v>44</v>
+      </c>
+      <c r="M2" t="s">
+        <v>47</v>
+      </c>
+      <c r="N2" t="s">
+        <v>51</v>
+      </c>
+      <c r="O2" t="s">
         <v>23</v>
       </c>
-      <c r="M2" t="s">
+      <c r="P2" t="s">
         <v>24</v>
       </c>
-      <c r="N2" t="s">
+      <c r="Q2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -850,17 +960,26 @@
         <v>1</v>
       </c>
       <c r="L3" t="s">
+        <v>46</v>
+      </c>
+      <c r="M3" t="s">
+        <v>48</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="O3" t="s">
         <v>30</v>
       </c>
-      <c r="M3" t="s">
+      <c r="P3" t="s">
         <v>31</v>
       </c>
-      <c r="N3" t="s">
+      <c r="Q3" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="4">
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576" xr:uid="{D995F1AB-73D8-4CCD-B7D1-2F71FF5E8915}">
       <formula1>"GenericDocument"</formula1>
     </dataValidation>
@@ -870,27 +989,30 @@
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:F1048576" xr:uid="{4D36C78B-754E-4CA0-B702-72B40F139561}">
       <formula1>18264</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K1:K1048576" xr:uid="{4E54745D-EA9D-492A-AE40-2899D961BCFA}">
-      <formula1>"1,2,3,4,5"</formula1>
-    </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="N3" r:id="rId1" display="mailto:NRSS_DataStore@nps.gov" xr:uid="{C148C2BF-F2AE-450D-81A8-0D73D2A6E6F7}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0591C5C5-FA56-4654-9944-818D77B92433}">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:L1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="5" max="5" width="18.6640625" customWidth="1"/>
     <col min="6" max="6" width="20.6640625" customWidth="1"/>
+    <col min="13" max="13" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -925,19 +1047,28 @@
         <v>11</v>
       </c>
       <c r="L1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M1" t="s">
+        <v>50</v>
+      </c>
+      <c r="N1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O1" t="s">
         <v>12</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>13</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>14</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -972,16 +1103,25 @@
         <v>1</v>
       </c>
       <c r="L2" t="s">
+        <v>44</v>
+      </c>
+      <c r="M2" t="s">
+        <v>47</v>
+      </c>
+      <c r="N2" t="s">
+        <v>51</v>
+      </c>
+      <c r="O2" t="s">
         <v>23</v>
       </c>
-      <c r="M2" t="s">
+      <c r="P2" t="s">
         <v>24</v>
       </c>
-      <c r="N2" t="s">
+      <c r="Q2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -1016,20 +1156,26 @@
         <v>1</v>
       </c>
       <c r="L3" t="s">
+        <v>46</v>
+      </c>
+      <c r="M3" t="s">
+        <v>48</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="O3" t="s">
         <v>30</v>
       </c>
-      <c r="M3" t="s">
+      <c r="P3" t="s">
         <v>31</v>
       </c>
-      <c r="N3" t="s">
+      <c r="Q3" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K1:K3" xr:uid="{F0505A24-7293-4103-8DBF-E1B56ABCAFED}">
-      <formula1>"1,2,3,4,5"</formula1>
-    </dataValidation>
+  <dataValidations count="3">
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:F3" xr:uid="{784B73C4-6D5A-4AA7-A042-5B500BF44D43}">
       <formula1>18264</formula1>
     </dataValidation>
@@ -1040,6 +1186,9 @@
       <formula1>"WebSite"</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="N3" r:id="rId1" display="mailto:NRSS_DataStore@nps.gov" xr:uid="{97C1C722-5CC9-4C2E-ACB9-8A2FA345DAE4}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updates to support owner lists and other additional information
</commit_message>
<xml_diff>
--- a/inst/extdata/DSbulkUploadR_input.xlsx
+++ b/inst/extdata/DSbulkUploadR_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rlbaker\Rdev_local\DSbulkUploadR\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F32EC832-CB93-4B6F-9267-B89AEA4BB086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{173C9A94-089D-4FF4-BC1F-8121E2B41F86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32565" yWindow="4605" windowWidth="21465" windowHeight="8880" activeTab="2" xr2:uid="{8A6EE447-C162-4970-95C2-F79FBBAD4C55}"/>
+    <workbookView xWindow="35580" yWindow="3510" windowWidth="17280" windowHeight="8880" xr2:uid="{8A6EE447-C162-4970-95C2-F79FBBAD4C55}"/>
   </bookViews>
   <sheets>
     <sheet name="AudioRecording" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="59">
   <si>
     <t>reference_type</t>
   </si>
@@ -209,6 +209,12 @@
   </si>
   <si>
     <t>NRSS, IMD</t>
+  </si>
+  <si>
+    <t>owner_email_list</t>
+  </si>
+  <si>
+    <t>sarah_wright@nps.gov</t>
   </si>
 </sst>
 </file>
@@ -592,10 +598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AA704E2-EB95-4E4A-95B2-36E8F6DDD1DD}">
-  <dimension ref="A1:S3"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:M1048576"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -606,13 +612,13 @@
     <col min="6" max="6" width="15.88671875" customWidth="1"/>
     <col min="8" max="8" width="10.21875" customWidth="1"/>
     <col min="10" max="10" width="6.33203125" customWidth="1"/>
-    <col min="11" max="11" width="11.6640625" customWidth="1"/>
-    <col min="12" max="12" width="11.77734375" customWidth="1"/>
-    <col min="14" max="14" width="10.6640625" customWidth="1"/>
-    <col min="18" max="18" width="9.21875" customWidth="1"/>
+    <col min="11" max="12" width="11.6640625" customWidth="1"/>
+    <col min="13" max="13" width="11.77734375" customWidth="1"/>
+    <col min="15" max="15" width="10.6640625" customWidth="1"/>
+    <col min="19" max="19" width="9.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -647,31 +653,34 @@
         <v>10</v>
       </c>
       <c r="L1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>45</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>50</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>49</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>13</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>14</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -705,29 +714,35 @@
       <c r="K2" t="s">
         <v>22</v>
       </c>
-      <c r="L2">
+      <c r="L2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2">
         <v>1</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>44</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>47</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>51</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>23</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>24</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>25</v>
       </c>
+      <c r="T2">
+        <v>2315517</v>
+      </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -761,26 +776,32 @@
       <c r="K3" t="s">
         <v>29</v>
       </c>
-      <c r="L3">
+      <c r="L3" t="s">
+        <v>58</v>
+      </c>
+      <c r="M3">
         <v>2</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>46</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>48</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="P3" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>56</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>31</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>32</v>
+      </c>
+      <c r="T3">
+        <v>2315517</v>
       </c>
     </row>
   </sheetData>
@@ -796,7 +817,7 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="O3" r:id="rId1" display="mailto:NRSS_DataStore@nps.gov" xr:uid="{3E3AFA6B-8503-44EF-BF3A-F5429543D37C}"/>
+    <hyperlink ref="P3" r:id="rId1" display="mailto:NRSS_DataStore@nps.gov" xr:uid="{3E3AFA6B-8503-44EF-BF3A-F5429543D37C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -804,19 +825,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32C372F4-B2F9-43E8-90EB-ACDD3F5DA605}">
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:N1048576"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="5" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.6640625" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" customWidth="1"/>
+    <col min="14" max="14" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -848,31 +870,34 @@
         <v>10</v>
       </c>
       <c r="K1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>45</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>50</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>49</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>12</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>14</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -903,29 +928,35 @@
       <c r="J2" t="s">
         <v>22</v>
       </c>
-      <c r="K2">
+      <c r="K2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2">
         <v>1</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>44</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>47</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>51</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>23</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>24</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>25</v>
       </c>
+      <c r="S2">
+        <v>2315517</v>
+      </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -956,26 +987,32 @@
       <c r="J3" t="s">
         <v>29</v>
       </c>
-      <c r="K3">
+      <c r="K3" t="s">
+        <v>58</v>
+      </c>
+      <c r="L3">
         <v>1</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>46</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>48</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>30</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>31</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>32</v>
+      </c>
+      <c r="S3">
+        <v>2315517</v>
       </c>
     </row>
   </sheetData>
@@ -991,7 +1028,7 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="N3" r:id="rId1" display="mailto:NRSS_DataStore@nps.gov" xr:uid="{C148C2BF-F2AE-450D-81A8-0D73D2A6E6F7}"/>
+    <hyperlink ref="O3" r:id="rId1" display="mailto:NRSS_DataStore@nps.gov" xr:uid="{C148C2BF-F2AE-450D-81A8-0D73D2A6E6F7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -999,20 +1036,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0591C5C5-FA56-4654-9944-818D77B92433}">
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="5" max="5" width="18.6640625" customWidth="1"/>
     <col min="6" max="6" width="20.6640625" customWidth="1"/>
-    <col min="13" max="13" width="10.6640625" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" customWidth="1"/>
+    <col min="14" max="14" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1044,31 +1082,34 @@
         <v>41</v>
       </c>
       <c r="K1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>45</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>50</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>49</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>12</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>14</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -1099,29 +1140,35 @@
       <c r="J2" t="s">
         <v>42</v>
       </c>
-      <c r="K2">
+      <c r="K2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2">
         <v>1</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>44</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>47</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>51</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>23</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>24</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>25</v>
       </c>
+      <c r="S2">
+        <v>2315517</v>
+      </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -1152,26 +1199,32 @@
       <c r="J3" t="s">
         <v>43</v>
       </c>
-      <c r="K3">
+      <c r="K3" t="s">
+        <v>58</v>
+      </c>
+      <c r="L3">
         <v>1</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>46</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>48</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>30</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>31</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>32</v>
+      </c>
+      <c r="S3">
+        <v>2315517</v>
       </c>
     </row>
   </sheetData>
@@ -1187,7 +1240,7 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="N3" r:id="rId1" display="mailto:NRSS_DataStore@nps.gov" xr:uid="{97C1C722-5CC9-4C2E-ACB9-8A2FA345DAE4}"/>
+    <hyperlink ref="O3" r:id="rId1" display="mailto:NRSS_DataStore@nps.gov" xr:uid="{97C1C722-5CC9-4C2E-ACB9-8A2FA345DAE4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add generic dataset sheet
</commit_message>
<xml_diff>
--- a/inst/extdata/DSbulkUploadR_input.xlsx
+++ b/inst/extdata/DSbulkUploadR_input.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rlbaker\Rdev_local\DSbulkUploadR\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{413F5747-EDB4-46CA-9F23-6754D81CE885}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C713A119-1FA4-44AA-98EE-47BB22E20ACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3060" yWindow="432" windowWidth="17280" windowHeight="8880" xr2:uid="{8A6EE447-C162-4970-95C2-F79FBBAD4C55}"/>
+    <workbookView xWindow="34200" yWindow="1485" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{8A6EE447-C162-4970-95C2-F79FBBAD4C55}"/>
   </bookViews>
   <sheets>
     <sheet name="AudioRecording" sheetId="1" r:id="rId1"/>
-    <sheet name="GenericDocument" sheetId="2" r:id="rId2"/>
-    <sheet name="WebSite" sheetId="3" r:id="rId3"/>
+    <sheet name="GenericDataset" sheetId="4" r:id="rId2"/>
+    <sheet name="GenericDocument" sheetId="2" r:id="rId3"/>
+    <sheet name="WebSite" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="66">
   <si>
     <t>reference_type</t>
   </si>
@@ -215,6 +216,27 @@
   </si>
   <si>
     <t>sarah_wright@nps.gov</t>
+  </si>
+  <si>
+    <t>GenericDataset</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Test GenericDataset</t>
+  </si>
+  <si>
+    <t>data for generic purposes</t>
+  </si>
+  <si>
+    <t>same as description</t>
+  </si>
+  <si>
+    <t>none of note</t>
+  </si>
+  <si>
+    <t>robert_baker@nps.gov, judd_patterson@nps.gov, daniel_wood@partner.nps.gov</t>
   </si>
 </sst>
 </file>
@@ -600,8 +622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AA704E2-EB95-4E4A-95B2-36E8F6DDD1DD}">
   <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2:T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -824,11 +846,163 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B81407D-D8D8-4DE4-AB2A-A11A6520C285}">
+  <dimension ref="A1:S2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+    <col min="4" max="4" width="5.77734375" customWidth="1"/>
+    <col min="5" max="5" width="17.77734375" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" customWidth="1"/>
+    <col min="10" max="10" width="16.21875" customWidth="1"/>
+    <col min="11" max="11" width="11.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N1" t="s">
+        <v>50</v>
+      </c>
+      <c r="O1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" t="s">
+        <v>14</v>
+      </c>
+      <c r="S1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" s="1">
+        <v>44975</v>
+      </c>
+      <c r="F2" s="1">
+        <v>45558</v>
+      </c>
+      <c r="G2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I2" t="s">
+        <v>64</v>
+      </c>
+      <c r="J2" t="s">
+        <v>65</v>
+      </c>
+      <c r="K2" t="s">
+        <v>58</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2" t="s">
+        <v>44</v>
+      </c>
+      <c r="N2" t="s">
+        <v>47</v>
+      </c>
+      <c r="O2" t="s">
+        <v>51</v>
+      </c>
+      <c r="P2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R2" t="s">
+        <v>25</v>
+      </c>
+      <c r="S2">
+        <v>2315517</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:F1" xr:uid="{0359E292-48B1-43E4-9592-D0B24B9C1221}">
+      <formula1>18264</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1" xr:uid="{6CA92E15-65A6-4B32-8336-E6CA9CF36627}">
+      <formula1>"Yes, No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1" xr:uid="{D022D274-EC99-429C-B9F4-CE39199B9D31}">
+      <formula1>"GenericDocument"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32C372F4-B2F9-43E8-90EB-ACDD3F5DA605}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1034,7 +1208,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0591C5C5-FA56-4654-9944-818D77B92433}">
   <dimension ref="A1:S3"/>
   <sheetViews>

</xml_diff>

<commit_message>
Add sheet for GenericDataset reference type
</commit_message>
<xml_diff>
--- a/inst/extdata/DSbulkUploadR_input.xlsx
+++ b/inst/extdata/DSbulkUploadR_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rlbaker\Rdev_local\DSbulkUploadR\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C713A119-1FA4-44AA-98EE-47BB22E20ACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50223138-D3E6-40CC-A33B-6A3DC6BB2E2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34200" yWindow="1485" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{8A6EE447-C162-4970-95C2-F79FBBAD4C55}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="18372" windowHeight="7104" activeTab="1" xr2:uid="{8A6EE447-C162-4970-95C2-F79FBBAD4C55}"/>
   </bookViews>
   <sheets>
     <sheet name="AudioRecording" sheetId="1" r:id="rId1"/>
@@ -236,7 +236,7 @@
     <t>none of note</t>
   </si>
   <si>
-    <t>robert_baker@nps.gov, judd_patterson@nps.gov, daniel_wood@partner.nps.gov</t>
+    <t>robert_baker@nps.gov, judd_patterson@nps.gov</t>
   </si>
 </sst>
 </file>
@@ -849,8 +849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B81407D-D8D8-4DE4-AB2A-A11A6520C285}">
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
setup Project data input sheet
</commit_message>
<xml_diff>
--- a/inst/extdata/DSbulkUploadR_input.xlsx
+++ b/inst/extdata/DSbulkUploadR_input.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rlbaker\Rdev_local\DSbulkUploadR\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50223138-D3E6-40CC-A33B-6A3DC6BB2E2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{629B41F5-9C57-45AC-8A28-714A9515AE71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="18372" windowHeight="7104" activeTab="1" xr2:uid="{8A6EE447-C162-4970-95C2-F79FBBAD4C55}"/>
+    <workbookView xWindow="2660" yWindow="2660" windowWidth="28800" windowHeight="15410" activeTab="4" xr2:uid="{8A6EE447-C162-4970-95C2-F79FBBAD4C55}"/>
   </bookViews>
   <sheets>
-    <sheet name="AudioRecording" sheetId="1" r:id="rId1"/>
-    <sheet name="GenericDataset" sheetId="4" r:id="rId2"/>
-    <sheet name="GenericDocument" sheetId="2" r:id="rId3"/>
+    <sheet name="GenericDataset" sheetId="4" r:id="rId1"/>
+    <sheet name="GenericDocument" sheetId="2" r:id="rId2"/>
+    <sheet name="AudioRecording" sheetId="1" r:id="rId3"/>
     <sheet name="WebSite" sheetId="3" r:id="rId4"/>
+    <sheet name="Project" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="70">
   <si>
     <t>reference_type</t>
   </si>
@@ -237,6 +238,18 @@
   </si>
   <si>
     <t>robert_baker@nps.gov, judd_patterson@nps.gov</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>stewards_email_list</t>
+  </si>
+  <si>
+    <t>leads_email_list</t>
+  </si>
+  <si>
+    <t>sponsors_email_list</t>
   </si>
 </sst>
 </file>
@@ -619,6 +632,369 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B81407D-D8D8-4DE4-AB2A-A11A6520C285}">
+  <dimension ref="A1:S2"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D1" sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.36328125" customWidth="1"/>
+    <col min="2" max="2" width="8.6328125" customWidth="1"/>
+    <col min="3" max="3" width="18.36328125" customWidth="1"/>
+    <col min="4" max="4" width="5.81640625" customWidth="1"/>
+    <col min="5" max="5" width="17.81640625" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
+    <col min="7" max="7" width="11.36328125" customWidth="1"/>
+    <col min="10" max="10" width="16.1796875" customWidth="1"/>
+    <col min="11" max="11" width="11.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N1" t="s">
+        <v>50</v>
+      </c>
+      <c r="O1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" t="s">
+        <v>14</v>
+      </c>
+      <c r="S1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" s="1">
+        <v>44975</v>
+      </c>
+      <c r="F2" s="1">
+        <v>45558</v>
+      </c>
+      <c r="G2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I2" t="s">
+        <v>64</v>
+      </c>
+      <c r="J2" t="s">
+        <v>65</v>
+      </c>
+      <c r="K2" t="s">
+        <v>58</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2" t="s">
+        <v>44</v>
+      </c>
+      <c r="N2" t="s">
+        <v>47</v>
+      </c>
+      <c r="O2" t="s">
+        <v>51</v>
+      </c>
+      <c r="P2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R2" t="s">
+        <v>25</v>
+      </c>
+      <c r="S2">
+        <v>2315517</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:F1" xr:uid="{0359E292-48B1-43E4-9592-D0B24B9C1221}">
+      <formula1>18264</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1" xr:uid="{6CA92E15-65A6-4B32-8336-E6CA9CF36627}">
+      <formula1>"Yes, No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1" xr:uid="{D022D274-EC99-429C-B9F4-CE39199B9D31}">
+      <formula1>"GenericDocument"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32C372F4-B2F9-43E8-90EB-ACDD3F5DA605}">
+  <dimension ref="A1:S3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="5" max="6" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.6328125" customWidth="1"/>
+    <col min="14" max="14" width="10.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N1" t="s">
+        <v>50</v>
+      </c>
+      <c r="O1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" t="s">
+        <v>14</v>
+      </c>
+      <c r="S1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="1">
+        <v>45644</v>
+      </c>
+      <c r="F2" s="1">
+        <v>45646</v>
+      </c>
+      <c r="G2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2" t="s">
+        <v>44</v>
+      </c>
+      <c r="N2" t="s">
+        <v>47</v>
+      </c>
+      <c r="O2" t="s">
+        <v>51</v>
+      </c>
+      <c r="P2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R2" t="s">
+        <v>25</v>
+      </c>
+      <c r="S2">
+        <v>2315517</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="1">
+        <v>45636</v>
+      </c>
+      <c r="F3" s="1">
+        <v>45635</v>
+      </c>
+      <c r="G3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" t="s">
+        <v>58</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3" t="s">
+        <v>46</v>
+      </c>
+      <c r="N3" t="s">
+        <v>48</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="P3" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>31</v>
+      </c>
+      <c r="R3" t="s">
+        <v>32</v>
+      </c>
+      <c r="S3">
+        <v>2315517</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576" xr:uid="{D995F1AB-73D8-4CCD-B7D1-2F71FF5E8915}">
+      <formula1>"GenericDocument"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576" xr:uid="{5B024554-7D2A-46C4-9639-8DBD487DE84E}">
+      <formula1>"Yes, No"</formula1>
+    </dataValidation>
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:F1048576" xr:uid="{4D36C78B-754E-4CA0-B702-72B40F139561}">
+      <formula1>18264</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="O3" r:id="rId1" display="mailto:NRSS_DataStore@nps.gov" xr:uid="{C148C2BF-F2AE-450D-81A8-0D73D2A6E6F7}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AA704E2-EB95-4E4A-95B2-36E8F6DDD1DD}">
   <dimension ref="A1:T3"/>
   <sheetViews>
@@ -626,21 +1002,21 @@
       <selection activeCell="N2" sqref="N2:T2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.21875" customWidth="1"/>
-    <col min="3" max="3" width="9.109375" customWidth="1"/>
-    <col min="5" max="5" width="17.44140625" customWidth="1"/>
-    <col min="6" max="6" width="15.88671875" customWidth="1"/>
-    <col min="8" max="8" width="10.21875" customWidth="1"/>
-    <col min="10" max="10" width="6.33203125" customWidth="1"/>
-    <col min="11" max="12" width="11.6640625" customWidth="1"/>
-    <col min="13" max="13" width="11.77734375" customWidth="1"/>
-    <col min="15" max="15" width="10.6640625" customWidth="1"/>
-    <col min="19" max="19" width="9.21875" customWidth="1"/>
+    <col min="1" max="1" width="13.1796875" customWidth="1"/>
+    <col min="3" max="3" width="9.08984375" customWidth="1"/>
+    <col min="5" max="5" width="17.453125" customWidth="1"/>
+    <col min="6" max="6" width="15.90625" customWidth="1"/>
+    <col min="8" max="8" width="10.1796875" customWidth="1"/>
+    <col min="10" max="10" width="6.36328125" customWidth="1"/>
+    <col min="11" max="12" width="11.6328125" customWidth="1"/>
+    <col min="13" max="13" width="11.81640625" customWidth="1"/>
+    <col min="15" max="15" width="10.6328125" customWidth="1"/>
+    <col min="19" max="19" width="9.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -702,7 +1078,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -764,7 +1140,7 @@
         <v>2315517</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -845,369 +1221,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B81407D-D8D8-4DE4-AB2A-A11A6520C285}">
-  <dimension ref="A1:S2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="14.33203125" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" customWidth="1"/>
-    <col min="4" max="4" width="5.77734375" customWidth="1"/>
-    <col min="5" max="5" width="17.77734375" customWidth="1"/>
-    <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" customWidth="1"/>
-    <col min="10" max="10" width="16.21875" customWidth="1"/>
-    <col min="11" max="11" width="11.5546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K1" t="s">
-        <v>57</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>45</v>
-      </c>
-      <c r="N1" t="s">
-        <v>50</v>
-      </c>
-      <c r="O1" t="s">
-        <v>49</v>
-      </c>
-      <c r="P1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>13</v>
-      </c>
-      <c r="R1" t="s">
-        <v>14</v>
-      </c>
-      <c r="S1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E2" s="1">
-        <v>44975</v>
-      </c>
-      <c r="F2" s="1">
-        <v>45558</v>
-      </c>
-      <c r="G2" t="s">
-        <v>62</v>
-      </c>
-      <c r="H2" t="s">
-        <v>63</v>
-      </c>
-      <c r="I2" t="s">
-        <v>64</v>
-      </c>
-      <c r="J2" t="s">
-        <v>65</v>
-      </c>
-      <c r="K2" t="s">
-        <v>58</v>
-      </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-      <c r="M2" t="s">
-        <v>44</v>
-      </c>
-      <c r="N2" t="s">
-        <v>47</v>
-      </c>
-      <c r="O2" t="s">
-        <v>51</v>
-      </c>
-      <c r="P2" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>24</v>
-      </c>
-      <c r="R2" t="s">
-        <v>25</v>
-      </c>
-      <c r="S2">
-        <v>2315517</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:F1" xr:uid="{0359E292-48B1-43E4-9592-D0B24B9C1221}">
-      <formula1>18264</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1" xr:uid="{6CA92E15-65A6-4B32-8336-E6CA9CF36627}">
-      <formula1>"Yes, No"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1" xr:uid="{D022D274-EC99-429C-B9F4-CE39199B9D31}">
-      <formula1>"GenericDocument"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32C372F4-B2F9-43E8-90EB-ACDD3F5DA605}">
-  <dimension ref="A1:S3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="A1:XFD1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="5" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.6640625" customWidth="1"/>
-    <col min="14" max="14" width="10.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K1" t="s">
-        <v>57</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>45</v>
-      </c>
-      <c r="N1" t="s">
-        <v>50</v>
-      </c>
-      <c r="O1" t="s">
-        <v>49</v>
-      </c>
-      <c r="P1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>13</v>
-      </c>
-      <c r="R1" t="s">
-        <v>14</v>
-      </c>
-      <c r="S1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" s="1">
-        <v>45644</v>
-      </c>
-      <c r="F2" s="1">
-        <v>45646</v>
-      </c>
-      <c r="G2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2" t="s">
-        <v>29</v>
-      </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-      <c r="M2" t="s">
-        <v>44</v>
-      </c>
-      <c r="N2" t="s">
-        <v>47</v>
-      </c>
-      <c r="O2" t="s">
-        <v>51</v>
-      </c>
-      <c r="P2" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>24</v>
-      </c>
-      <c r="R2" t="s">
-        <v>25</v>
-      </c>
-      <c r="S2">
-        <v>2315517</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="1">
-        <v>45636</v>
-      </c>
-      <c r="F3" s="1">
-        <v>45635</v>
-      </c>
-      <c r="G3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" t="s">
-        <v>29</v>
-      </c>
-      <c r="K3" t="s">
-        <v>58</v>
-      </c>
-      <c r="L3">
-        <v>1</v>
-      </c>
-      <c r="M3" t="s">
-        <v>46</v>
-      </c>
-      <c r="N3" t="s">
-        <v>48</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="P3" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>31</v>
-      </c>
-      <c r="R3" t="s">
-        <v>32</v>
-      </c>
-      <c r="S3">
-        <v>2315517</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576" xr:uid="{D995F1AB-73D8-4CCD-B7D1-2F71FF5E8915}">
-      <formula1>"GenericDocument"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576" xr:uid="{5B024554-7D2A-46C4-9639-8DBD487DE84E}">
-      <formula1>"Yes, No"</formula1>
-    </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:F1048576" xr:uid="{4D36C78B-754E-4CA0-B702-72B40F139561}">
-      <formula1>18264</formula1>
-    </dataValidation>
-  </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="O3" r:id="rId1" display="mailto:NRSS_DataStore@nps.gov" xr:uid="{C148C2BF-F2AE-450D-81A8-0D73D2A6E6F7}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0591C5C5-FA56-4654-9944-818D77B92433}">
   <dimension ref="A1:S3"/>
@@ -1216,15 +1229,15 @@
       <selection activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" width="18.6640625" customWidth="1"/>
-    <col min="6" max="6" width="20.6640625" customWidth="1"/>
-    <col min="11" max="11" width="11.6640625" customWidth="1"/>
-    <col min="14" max="14" width="10.6640625" customWidth="1"/>
+    <col min="5" max="5" width="18.6328125" customWidth="1"/>
+    <col min="6" max="6" width="20.6328125" customWidth="1"/>
+    <col min="11" max="11" width="11.6328125" customWidth="1"/>
+    <col min="14" max="14" width="10.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1283,7 +1296,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -1342,7 +1355,7 @@
         <v>2315517</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -1418,4 +1431,91 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36F8CC3E-9092-4E88-8E6A-27D4AA288ABA}">
+  <dimension ref="A1:R2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N1" t="s">
+        <v>50</v>
+      </c>
+      <c r="O1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1" xr:uid="{EB211272-910D-4987-85E2-04583C1EE0CB}">
+      <formula1>"GenericDocument"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1" xr:uid="{4F6100E9-CD6E-492E-841E-2836B1C34381}">
+      <formula1>"Yes, No"</formula1>
+    </dataValidation>
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1" xr:uid="{8E582D2C-63A3-4AB1-BD31-039C1F749E66}">
+      <formula1>18264</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add data validation for Project and GenericDataset Reference columns
</commit_message>
<xml_diff>
--- a/inst/extdata/DSbulkUploadR_input.xlsx
+++ b/inst/extdata/DSbulkUploadR_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rlbaker\Rdev_local\DSbulkUploadR\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{629B41F5-9C57-45AC-8A28-714A9515AE71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD9EE765-C5F8-4FB0-8B83-75A67580BE15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2660" yWindow="2660" windowWidth="28800" windowHeight="15410" activeTab="4" xr2:uid="{8A6EE447-C162-4970-95C2-F79FBBAD4C55}"/>
+    <workbookView xWindow="9230" yWindow="4180" windowWidth="28120" windowHeight="15410" xr2:uid="{8A6EE447-C162-4970-95C2-F79FBBAD4C55}"/>
   </bookViews>
   <sheets>
     <sheet name="GenericDataset" sheetId="4" r:id="rId1"/>
@@ -635,8 +635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B81407D-D8D8-4DE4-AB2A-A11A6520C285}">
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D1" sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -775,8 +775,8 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1" xr:uid="{6CA92E15-65A6-4B32-8336-E6CA9CF36627}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1" xr:uid="{D022D274-EC99-429C-B9F4-CE39199B9D31}">
-      <formula1>"GenericDocument"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A2" xr:uid="{D022D274-EC99-429C-B9F4-CE39199B9D31}">
+      <formula1>"GenericDataset"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -788,7 +788,7 @@
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="A1:XFD1"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -998,8 +998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AA704E2-EB95-4E4A-95B2-36E8F6DDD1DD}">
   <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2:T2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1226,7 +1226,7 @@
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K1048576"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1437,8 +1437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36F8CC3E-9092-4E88-8E6A-27D4AA288ABA}">
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1506,8 +1506,8 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1" xr:uid="{EB211272-910D-4987-85E2-04583C1EE0CB}">
-      <formula1>"GenericDocument"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A2" xr:uid="{EB211272-910D-4987-85E2-04583C1EE0CB}">
+      <formula1>"Project"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1" xr:uid="{4F6100E9-CD6E-492E-841E-2836B1C34381}">
       <formula1>"Yes, No"</formula1>

</xml_diff>

<commit_message>
Add a page for FieldNotes reference type. n.b. FieldNotes is not a real reference type and does not exist on DataStore.
</commit_message>
<xml_diff>
--- a/inst/extdata/DSbulkUploadR_input.xlsx
+++ b/inst/extdata/DSbulkUploadR_input.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rlbaker\Rdev_local\DSbulkUploadR\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD9EE765-C5F8-4FB0-8B83-75A67580BE15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DF49F59-98D3-4955-B280-FB81E4BEF9E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9230" yWindow="4180" windowWidth="28120" windowHeight="15410" xr2:uid="{8A6EE447-C162-4970-95C2-F79FBBAD4C55}"/>
+    <workbookView xWindow="29685" yWindow="750" windowWidth="24615" windowHeight="13275" activeTab="1" xr2:uid="{8A6EE447-C162-4970-95C2-F79FBBAD4C55}"/>
   </bookViews>
   <sheets>
     <sheet name="GenericDataset" sheetId="4" r:id="rId1"/>
-    <sheet name="GenericDocument" sheetId="2" r:id="rId2"/>
-    <sheet name="AudioRecording" sheetId="1" r:id="rId3"/>
-    <sheet name="WebSite" sheetId="3" r:id="rId4"/>
-    <sheet name="Project" sheetId="5" r:id="rId5"/>
+    <sheet name="FieldNotes" sheetId="6" r:id="rId2"/>
+    <sheet name="GenericDocument" sheetId="2" r:id="rId3"/>
+    <sheet name="AudioRecording" sheetId="1" r:id="rId4"/>
+    <sheet name="WebSite" sheetId="3" r:id="rId5"/>
+    <sheet name="Project" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="71">
   <si>
     <t>reference_type</t>
   </si>
@@ -250,6 +251,9 @@
   </si>
   <si>
     <t>sponsors_email_list</t>
+  </si>
+  <si>
+    <t>FieldNotes</t>
   </si>
 </sst>
 </file>
@@ -635,24 +639,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B81407D-D8D8-4DE4-AB2A-A11A6520C285}">
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.36328125" customWidth="1"/>
-    <col min="2" max="2" width="8.6328125" customWidth="1"/>
-    <col min="3" max="3" width="18.36328125" customWidth="1"/>
-    <col min="4" max="4" width="5.81640625" customWidth="1"/>
-    <col min="5" max="5" width="17.81640625" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+    <col min="4" max="4" width="5.77734375" customWidth="1"/>
+    <col min="5" max="5" width="17.77734375" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="7" width="11.36328125" customWidth="1"/>
-    <col min="10" max="10" width="16.1796875" customWidth="1"/>
-    <col min="11" max="11" width="11.54296875" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" customWidth="1"/>
+    <col min="10" max="10" width="16.21875" customWidth="1"/>
+    <col min="11" max="11" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -711,7 +715,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>59</v>
       </c>
@@ -784,6 +788,147 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02740E3C-2CB5-4540-B9FC-9B8FBF6E48A3}">
+  <dimension ref="A1:S2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N1" t="s">
+        <v>50</v>
+      </c>
+      <c r="O1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" t="s">
+        <v>14</v>
+      </c>
+      <c r="S1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" s="1">
+        <v>44975</v>
+      </c>
+      <c r="F2" s="1">
+        <v>45558</v>
+      </c>
+      <c r="G2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I2" t="s">
+        <v>64</v>
+      </c>
+      <c r="J2" t="s">
+        <v>65</v>
+      </c>
+      <c r="K2" t="s">
+        <v>58</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2" t="s">
+        <v>44</v>
+      </c>
+      <c r="N2" t="s">
+        <v>47</v>
+      </c>
+      <c r="O2" t="s">
+        <v>51</v>
+      </c>
+      <c r="P2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R2" t="s">
+        <v>25</v>
+      </c>
+      <c r="S2">
+        <v>2315517</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1" xr:uid="{D25A4B78-251F-4041-A15B-308ADE4ACC73}">
+      <formula1>"Yes, No"</formula1>
+    </dataValidation>
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:F1" xr:uid="{3FFDB4EB-46D3-48E3-BFAF-C9F84595E7CE}">
+      <formula1>18264</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A2" xr:uid="{4C1E8518-3C7F-4113-8E0E-15FBD22F16CE}">
+      <formula1>"FieldNotes"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32C372F4-B2F9-43E8-90EB-ACDD3F5DA605}">
   <dimension ref="A1:S3"/>
   <sheetViews>
@@ -791,14 +936,14 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="6" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.6328125" customWidth="1"/>
-    <col min="14" max="14" width="10.6328125" customWidth="1"/>
+    <col min="5" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" customWidth="1"/>
+    <col min="14" max="14" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -857,7 +1002,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -916,7 +1061,7 @@
         <v>2315517</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -994,7 +1139,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AA704E2-EB95-4E4A-95B2-36E8F6DDD1DD}">
   <dimension ref="A1:T3"/>
   <sheetViews>
@@ -1002,21 +1147,21 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.1796875" customWidth="1"/>
-    <col min="3" max="3" width="9.08984375" customWidth="1"/>
-    <col min="5" max="5" width="17.453125" customWidth="1"/>
-    <col min="6" max="6" width="15.90625" customWidth="1"/>
-    <col min="8" max="8" width="10.1796875" customWidth="1"/>
-    <col min="10" max="10" width="6.36328125" customWidth="1"/>
-    <col min="11" max="12" width="11.6328125" customWidth="1"/>
-    <col min="13" max="13" width="11.81640625" customWidth="1"/>
-    <col min="15" max="15" width="10.6328125" customWidth="1"/>
-    <col min="19" max="19" width="9.1796875" customWidth="1"/>
+    <col min="1" max="1" width="13.21875" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" customWidth="1"/>
+    <col min="8" max="8" width="10.21875" customWidth="1"/>
+    <col min="10" max="10" width="6.33203125" customWidth="1"/>
+    <col min="11" max="12" width="11.6640625" customWidth="1"/>
+    <col min="13" max="13" width="11.77734375" customWidth="1"/>
+    <col min="15" max="15" width="10.6640625" customWidth="1"/>
+    <col min="19" max="19" width="9.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1078,7 +1223,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -1140,7 +1285,7 @@
         <v>2315517</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1221,7 +1366,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0591C5C5-FA56-4654-9944-818D77B92433}">
   <dimension ref="A1:S3"/>
   <sheetViews>
@@ -1229,15 +1374,15 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="18.6328125" customWidth="1"/>
-    <col min="6" max="6" width="20.6328125" customWidth="1"/>
-    <col min="11" max="11" width="11.6328125" customWidth="1"/>
-    <col min="14" max="14" width="10.6328125" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" customWidth="1"/>
+    <col min="14" max="14" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1296,7 +1441,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -1355,7 +1500,7 @@
         <v>2315517</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -1433,7 +1578,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36F8CC3E-9092-4E88-8E6A-27D4AA288ABA}">
   <dimension ref="A1:R2"/>
   <sheetViews>
@@ -1441,9 +1586,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1499,7 +1644,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>66</v>
       </c>

</xml_diff>

<commit_message>
add Script sheet to input.xlsx
</commit_message>
<xml_diff>
--- a/inst/extdata/DSbulkUploadR_input.xlsx
+++ b/inst/extdata/DSbulkUploadR_input.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rlbaker\Rdev_local\DSbulkUploadR\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{344BEF19-5813-4B37-B8EC-FB0ADE95CBE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3C933D8-8279-4F7D-94C2-67446046486F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29685" yWindow="750" windowWidth="24615" windowHeight="13275" activeTab="1" xr2:uid="{8A6EE447-C162-4970-95C2-F79FBBAD4C55}"/>
+    <workbookView xWindow="30270" yWindow="1515" windowWidth="24615" windowHeight="13275" activeTab="5" xr2:uid="{8A6EE447-C162-4970-95C2-F79FBBAD4C55}"/>
   </bookViews>
   <sheets>
-    <sheet name="GenericDataset" sheetId="4" r:id="rId1"/>
-    <sheet name="FieldNotes" sheetId="6" r:id="rId2"/>
-    <sheet name="GenericDocument" sheetId="2" r:id="rId3"/>
-    <sheet name="AudioRecording" sheetId="1" r:id="rId4"/>
-    <sheet name="WebSite" sheetId="3" r:id="rId5"/>
-    <sheet name="Project" sheetId="5" r:id="rId6"/>
+    <sheet name="Project" sheetId="5" r:id="rId1"/>
+    <sheet name="GenericDataset" sheetId="4" r:id="rId2"/>
+    <sheet name="FieldNotes" sheetId="6" r:id="rId3"/>
+    <sheet name="GenericDocument" sheetId="2" r:id="rId4"/>
+    <sheet name="AudioRecording" sheetId="1" r:id="rId5"/>
+    <sheet name="Script" sheetId="7" r:id="rId6"/>
+    <sheet name="WebSite" sheetId="3" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="85">
   <si>
     <t>reference_type</t>
   </si>
@@ -269,6 +270,33 @@
   </si>
   <si>
     <t>Test FieldNotes3</t>
+  </si>
+  <si>
+    <t>Script</t>
+  </si>
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>scripting_language</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>python</t>
+  </si>
+  <si>
+    <t>0.0.1</t>
+  </si>
+  <si>
+    <t>1.1.0</t>
+  </si>
+  <si>
+    <t>steward_email</t>
+  </si>
+  <si>
+    <t>Data Monkey</t>
   </si>
 </sst>
 </file>
@@ -651,6 +679,93 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36F8CC3E-9092-4E88-8E6A-27D4AA288ABA}">
+  <dimension ref="A1:R2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N1" t="s">
+        <v>50</v>
+      </c>
+      <c r="O1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A2" xr:uid="{EB211272-910D-4987-85E2-04583C1EE0CB}">
+      <formula1>"Project"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1" xr:uid="{4F6100E9-CD6E-492E-841E-2836B1C34381}">
+      <formula1>"Yes, No"</formula1>
+    </dataValidation>
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1" xr:uid="{8E582D2C-63A3-4AB1-BD31-039C1F749E66}">
+      <formula1>18264</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B81407D-D8D8-4DE4-AB2A-A11A6520C285}">
   <dimension ref="A1:S2"/>
   <sheetViews>
@@ -802,11 +917,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02740E3C-2CB5-4540-B9FC-9B8FBF6E48A3}">
   <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
@@ -1064,12 +1179,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32C372F4-B2F9-43E8-90EB-ACDD3F5DA605}">
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1275,7 +1390,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AA704E2-EB95-4E4A-95B2-36E8F6DDD1DD}">
   <dimension ref="A1:T3"/>
   <sheetViews>
@@ -1502,7 +1617,222 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D704E2B-E668-4D16-AAE0-B58A99B5B51C}">
+  <dimension ref="A1:T3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>83</v>
+      </c>
+      <c r="L1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O1" t="s">
+        <v>50</v>
+      </c>
+      <c r="P1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1" t="s">
+        <v>14</v>
+      </c>
+      <c r="T1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" t="s">
+        <v>58</v>
+      </c>
+      <c r="L2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2" t="s">
+        <v>44</v>
+      </c>
+      <c r="O2" t="s">
+        <v>47</v>
+      </c>
+      <c r="P2" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>23</v>
+      </c>
+      <c r="R2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S2" t="s">
+        <v>25</v>
+      </c>
+      <c r="T2">
+        <v>2315517</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" t="s">
+        <v>29</v>
+      </c>
+      <c r="L3" t="s">
+        <v>58</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3" t="s">
+        <v>46</v>
+      </c>
+      <c r="O3" t="s">
+        <v>84</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>30</v>
+      </c>
+      <c r="R3" t="s">
+        <v>31</v>
+      </c>
+      <c r="S3" t="s">
+        <v>32</v>
+      </c>
+      <c r="T3">
+        <v>2315517</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C3" xr:uid="{0E11573E-BFDF-4090-ADE3-ACEE7B1130EA}">
+      <formula1>"Yes, No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576" xr:uid="{3C490254-272D-499A-BB89-7E62B524A514}">
+      <formula1>"Script"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="P3" r:id="rId1" display="mailto:NRSS_DataStore@nps.gov" xr:uid="{B81D948F-3067-40F8-99D2-80172FE813C2}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0591C5C5-FA56-4654-9944-818D77B92433}">
   <dimension ref="A1:S3"/>
   <sheetViews>
@@ -1712,91 +2042,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36F8CC3E-9092-4E88-8E6A-27D4AA288ABA}">
-  <dimension ref="A1:R2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" t="s">
-        <v>68</v>
-      </c>
-      <c r="I1" t="s">
-        <v>67</v>
-      </c>
-      <c r="J1" t="s">
-        <v>69</v>
-      </c>
-      <c r="K1" t="s">
-        <v>57</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>45</v>
-      </c>
-      <c r="N1" t="s">
-        <v>50</v>
-      </c>
-      <c r="O1" t="s">
-        <v>49</v>
-      </c>
-      <c r="P1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>13</v>
-      </c>
-      <c r="R1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A2" xr:uid="{EB211272-910D-4987-85E2-04583C1EE0CB}">
-      <formula1>"Project"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1" xr:uid="{4F6100E9-CD6E-492E-841E-2836B1C34381}">
-      <formula1>"Yes, No"</formula1>
-    </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1" xr:uid="{8E582D2C-63A3-4AB1-BD31-039C1F749E66}">
-      <formula1>18264</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
update for script references
</commit_message>
<xml_diff>
--- a/inst/extdata/DSbulkUploadR_input.xlsx
+++ b/inst/extdata/DSbulkUploadR_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rlbaker\Rdev_local\DSbulkUploadR\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3C933D8-8279-4F7D-94C2-67446046486F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1AFAA7D-F788-49C2-93D6-C635CA922A44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30270" yWindow="1515" windowWidth="24615" windowHeight="13275" activeTab="5" xr2:uid="{8A6EE447-C162-4970-95C2-F79FBBAD4C55}"/>
+    <workbookView xWindow="29580" yWindow="2205" windowWidth="24615" windowHeight="13275" activeTab="5" xr2:uid="{8A6EE447-C162-4970-95C2-F79FBBAD4C55}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="5" r:id="rId1"/>
@@ -1622,7 +1622,7 @@
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+      <selection activeCell="N1" sqref="N1:N1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
update: "owner" changed to "editor" to match datastore v4.0.0
</commit_message>
<xml_diff>
--- a/inst/extdata/DSbulkUploadR_input.xlsx
+++ b/inst/extdata/DSbulkUploadR_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rlbaker\Rdev_local\DSbulkUploadR\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1AFAA7D-F788-49C2-93D6-C635CA922A44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB9DE21A-3122-4D2E-8FD5-0056D32C01F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29580" yWindow="2205" windowWidth="24615" windowHeight="13275" activeTab="5" xr2:uid="{8A6EE447-C162-4970-95C2-F79FBBAD4C55}"/>
+    <workbookView xWindow="29580" yWindow="2400" windowWidth="26130" windowHeight="8475" activeTab="6" xr2:uid="{8A6EE447-C162-4970-95C2-F79FBBAD4C55}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="5" r:id="rId1"/>
@@ -215,9 +215,6 @@
     <t>NRSS, IMD</t>
   </si>
   <si>
-    <t>owner_email_list</t>
-  </si>
-  <si>
     <t>sarah_wright@nps.gov</t>
   </si>
   <si>
@@ -297,6 +294,9 @@
   </si>
   <si>
     <t>Data Monkey</t>
+  </si>
+  <si>
+    <t>editor_email_list</t>
   </si>
 </sst>
 </file>
@@ -683,7 +683,7 @@
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -711,16 +711,16 @@
         <v>9</v>
       </c>
       <c r="H1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J1" t="s">
         <v>68</v>
       </c>
-      <c r="I1" t="s">
-        <v>67</v>
-      </c>
-      <c r="J1" t="s">
-        <v>69</v>
-      </c>
       <c r="K1" t="s">
-        <v>57</v>
+        <v>84</v>
       </c>
       <c r="L1" t="s">
         <v>11</v>
@@ -746,7 +746,7 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -770,7 +770,7 @@
   <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -818,7 +818,7 @@
         <v>10</v>
       </c>
       <c r="K1" t="s">
-        <v>57</v>
+        <v>84</v>
       </c>
       <c r="L1" t="s">
         <v>11</v>
@@ -847,13 +847,13 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" t="s">
         <v>59</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>60</v>
-      </c>
-      <c r="D2" t="s">
-        <v>61</v>
       </c>
       <c r="E2" s="1">
         <v>44975</v>
@@ -862,19 +862,19 @@
         <v>45558</v>
       </c>
       <c r="G2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H2" t="s">
         <v>62</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>63</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>64</v>
       </c>
-      <c r="J2" t="s">
-        <v>65</v>
-      </c>
       <c r="K2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L2">
         <v>1</v>
@@ -922,7 +922,7 @@
   <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -959,7 +959,7 @@
         <v>10</v>
       </c>
       <c r="K1" t="s">
-        <v>57</v>
+        <v>84</v>
       </c>
       <c r="L1" t="s">
         <v>11</v>
@@ -988,16 +988,16 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B2" t="s">
         <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E2" s="1">
         <v>44975</v>
@@ -1006,19 +1006,19 @@
         <v>45558</v>
       </c>
       <c r="G2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H2" t="s">
         <v>62</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>63</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>64</v>
       </c>
-      <c r="J2" t="s">
-        <v>65</v>
-      </c>
       <c r="K2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L2">
         <v>1</v>
@@ -1047,16 +1047,16 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E3" s="1">
         <v>44975</v>
@@ -1065,19 +1065,19 @@
         <v>45558</v>
       </c>
       <c r="G3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H3" t="s">
         <v>62</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>63</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>64</v>
       </c>
-      <c r="J3" t="s">
-        <v>65</v>
-      </c>
       <c r="K3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L3">
         <v>1</v>
@@ -1106,16 +1106,16 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E4" s="1">
         <v>44975</v>
@@ -1124,19 +1124,19 @@
         <v>45558</v>
       </c>
       <c r="G4" t="s">
+        <v>61</v>
+      </c>
+      <c r="H4" t="s">
         <v>62</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>63</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>64</v>
       </c>
-      <c r="J4" t="s">
-        <v>65</v>
-      </c>
       <c r="K4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L4">
         <v>1</v>
@@ -1184,7 +1184,7 @@
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD3"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1226,7 +1226,7 @@
         <v>10</v>
       </c>
       <c r="K1" t="s">
-        <v>57</v>
+        <v>84</v>
       </c>
       <c r="L1" t="s">
         <v>11</v>
@@ -1344,7 +1344,7 @@
         <v>29</v>
       </c>
       <c r="K3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L3">
         <v>1</v>
@@ -1395,7 +1395,7 @@
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1447,7 +1447,7 @@
         <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>57</v>
+        <v>84</v>
       </c>
       <c r="M1" t="s">
         <v>11</v>
@@ -1571,7 +1571,7 @@
         <v>29</v>
       </c>
       <c r="L3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M3">
         <v>2</v>
@@ -1621,8 +1621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D704E2B-E668-4D16-AAE0-B58A99B5B51C}">
   <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:N1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1644,10 +1644,10 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" t="s">
         <v>77</v>
-      </c>
-      <c r="F1" t="s">
-        <v>78</v>
       </c>
       <c r="G1" t="s">
         <v>7</v>
@@ -1662,10 +1662,10 @@
         <v>10</v>
       </c>
       <c r="K1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L1" t="s">
-        <v>57</v>
+        <v>84</v>
       </c>
       <c r="M1" t="s">
         <v>11</v>
@@ -1694,7 +1694,7 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B2" t="s">
         <v>16</v>
@@ -1706,10 +1706,10 @@
         <v>34</v>
       </c>
       <c r="E2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G2" t="s">
         <v>33</v>
@@ -1724,7 +1724,7 @@
         <v>22</v>
       </c>
       <c r="K2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L2" t="s">
         <v>29</v>
@@ -1756,7 +1756,7 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
@@ -1768,10 +1768,10 @@
         <v>35</v>
       </c>
       <c r="E3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G3" t="s">
         <v>33</v>
@@ -1789,7 +1789,7 @@
         <v>29</v>
       </c>
       <c r="L3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M3">
         <v>1</v>
@@ -1798,7 +1798,7 @@
         <v>46</v>
       </c>
       <c r="O3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="P3" s="2" t="s">
         <v>52</v>
@@ -1836,8 +1836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0591C5C5-FA56-4654-9944-818D77B92433}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1880,7 +1880,7 @@
         <v>41</v>
       </c>
       <c r="K1" t="s">
-        <v>57</v>
+        <v>84</v>
       </c>
       <c r="L1" t="s">
         <v>11</v>
@@ -1998,7 +1998,7 @@
         <v>43</v>
       </c>
       <c r="K3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L3">
         <v>1</v>

</xml_diff>